<commit_message>
Plot function changes for 16 users and thesis consolidated results excel
</commit_message>
<xml_diff>
--- a/Thesis_consolidated_results.xlsx
+++ b/Thesis_consolidated_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijan\Documents\SXRSIMv3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4A6BA9-29DF-474A-8519-B5A185B8D251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAEA95A-A790-4797-B58A-718BB524D6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{430AC486-BDEE-4081-8A97-82598AAF22D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{430AC486-BDEE-4081-8A97-82598AAF22D1}"/>
   </bookViews>
   <sheets>
     <sheet name="4 UEs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>SEED</t>
   </si>
@@ -78,9 +78,6 @@
     <t>3.5 GHz</t>
   </si>
   <si>
-    <t>[103.1427731581173, 100.0765478424015, 100.0765478424015, 108.6112600536193]</t>
-  </si>
-  <si>
     <t>More collisions between UE0 and 15</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Average BLER (%)</t>
   </si>
   <si>
-    <t>[103.02771783316471, 100.07654772732958, 100.0765347942464, 250.05723205697814]</t>
-  </si>
-  <si>
     <t>[0.4314969802875624, 0.006253908692933082, 0.32958098811757347, 0.09241987451246396]</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>We expect to see all Ues scheduled all times, but here the interference will be higher making the SINR lower and hence bitrate should reduce. What will happen to PLR? How can we logically back that?</t>
   </si>
   <si>
-    <t>[24.75422658939163, 100.07654761225766, 100.07644209130706, 66.82017495140079]</t>
-  </si>
-  <si>
     <t>[0.281986104050161, 0.008338544923910776, 0.4318323952470294, 0.269916142557652]</t>
   </si>
   <si>
@@ -132,9 +123,6 @@
     <t>[0.43250244171727037, 1.4536430771070648, 0.10287679799874921, 1.1726063048314652, 0.3499951245673053, 0.7660810245519194, 0.1711514392991239, 1.1337342855949546, 0.30764844620687865, 0.6765993098962638, 0.046910182636977736, 0.7502356558960332, 0.01516357708783502, 0.7742036227357901, 0.028142589118198873, 0.5982730731551728]</t>
   </si>
   <si>
-    <t>[89.75365088963437, 210.0975235805902, 100.07654268918074, 143.3507552701171, 89.37385917800204, 122.1938486726518, 100.13915812265334, 253.84719699285804, 86.19942716740533, 105.7020342494295, 100.08906094570928, 132.70926495758192, 79.5676224269305, 156.63083927545284, 100.07654484052533, 109.11763537693936]</t>
-  </si>
-  <si>
     <t>Bandwidth (MHz)</t>
   </si>
   <si>
@@ -144,9 +132,6 @@
     <t>[2.573449401523395, 3.3569762922658377, 0.4625336205532634, 4.091287322564855, 1.351976558885519, 4.033737307566328, 0.6120395892211251, 3.048089670965409, 2.1725239616613417, 2.080581343432944, 0.22769439232853866, 2.921579408231005, 2.2202293254756262, 2.962408617915979, 0.08005003126954346, 2.8714152088681915]</t>
   </si>
   <si>
-    <t>[92.53830937008826, 190.1437457183573, 112.96577899156597, 218.70945873715124, 85.23285757466714, 197.65330567965933, 110.2235594291895, 189.89563480776184, 91.64186395585244, 147.81975265807586, 99.15600135084428, 194.22409378703645, 76.21066709371597, 194.6890213940986, 100.07652412757975, 191.1615802256851]</t>
-  </si>
-  <si>
     <t>WELL YES OFCOURSE!! With Ls = 1, the collisions are going to be head on! Changing gamma doesn’t matter at all unless you keep gamma as 0.99 or 1!</t>
   </si>
   <si>
@@ -198,16 +183,46 @@
     <t>[2.6531487380543983, 4.279083631408619, 0.5149061464850938, 5.132844401461423, 1.5187759830982075, 6.487526427061311, 0.8179488131941607, 3.683048822469271, 3.844891614129027, 3.0131744383097354, 0.24060248426955302, 3.3159190536239715, 2.7533111502577152, 3.3755679657319, 0.13570014713198478, 3.584786291792661]</t>
   </si>
   <si>
-    <t>[97.07843646165155, 197.56367399080224, 114.10238607287448, 251.28535480335267, 93.75292304232264, 263.84440382241013, 117.00970599903421, 193.4994878075451, 88.88821556265651, 174.965112731646, 104.24269602582075, 190.34014714465863, 79.63865596659488, 191.86129970575874, 101.66494940141628, 205.7297662999421]</t>
-  </si>
-  <si>
     <t>Bitrate has increased for some Ues and PLR has reduced mildly. I don’t think reducing gamma any below is going to help considering th collisions.</t>
   </si>
   <si>
-    <t>Please simulate with lesser bandwidth and repeat the same as well, the gamma I mean.</t>
-  </si>
-  <si>
-    <t>Check if BW affects PLR please, reducing gamma can no longer bring down PLR.</t>
+    <t>Fix bitrate please, you need to average over entire TTI and not just the TTIs where they are scheduled.</t>
+  </si>
+  <si>
+    <t>[42.28351812883052, 100.07654773733583, 100.07652794496559, 100.04780322201375]</t>
+  </si>
+  <si>
+    <t>[70.05755947467166, 100.07654772732958, 100.0765347942464, 92.21935568730457]</t>
+  </si>
+  <si>
+    <t>You keep same gamma but increase L, now in the places where there are collisions, there is no head-on collision, due to LC the overlap reduces and spreads out due to which interference reduces, SINR improves, bitrate improves and PLR decreases.</t>
+  </si>
+  <si>
+    <t>[22.838444512820516, 100.07654761225766, 100.07644209130706, 58.47078723702313]</t>
+  </si>
+  <si>
+    <t>Within same Ls, if we increase gamma, we allow more Ues to be co-scheduled but at the expense of higher interfernce and hence SINR decreases and the bitrate and also PLR increases.</t>
+  </si>
+  <si>
+    <t>Final explanation</t>
+  </si>
+  <si>
+    <t>Indeed those values are coming, maybe because of an orientation difference that is taking place.</t>
+  </si>
+  <si>
+    <t>[66.09157988742965, 73.24506849280802, 100.07654268918074, 71.1912662664165, 76.42890246404002, 79.16235637273296, 100.07653200750471, 63.35067164477798, 69.33150924327704, 99.94097590994372, 100.07654198874296, 89.5144325953721, 65.63209230769229, 78.41337513445905, 100.07654484052533, 99.84365998749217]</t>
+  </si>
+  <si>
+    <t>[47.86643882426516, 91.78984197623515, 96.74858414008756, 93.14642989368355, 51.84599056910568, 94.3457695809881, 98.78416000000001, 98.53433908692932, 29.598774634146338, 100.07646856785492, 99.15600135084428, 99.41382711694808, 37.202148968105064, 99.65180085053159, 100.07652412757975, 100.1177394371482]</t>
+  </si>
+  <si>
+    <t>For some Ues, the level of interfernce can reduce when there are 2 precoders combined, for some which had no interference previously , there can be more with 2 beams, so the result here highly depends on the precoder selection.</t>
+  </si>
+  <si>
+    <t>[49.55310809255785, 96.7184765478424, 96.94064507817386, 97.49683184490306, 57.354039599749846, 97.55972717948717, 98.49963399624765, 99.59959564727956, 32.183760100062536, 100.08245175734835, 99.98237070669168, 99.11614979362102, 38.16828267667291, 99.90826216385241, 100.11041030644152, 99.98929823639776]</t>
+  </si>
+  <si>
+    <t>With the correct gamma, LS = 2, will be better than Ls = 1</t>
   </si>
 </sst>
 </file>
@@ -231,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +280,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -327,19 +348,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -348,6 +360,32 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -664,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB69F719-4A6A-4C2B-9A98-580430B71420}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,15 +722,16 @@
     <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.44140625" customWidth="1"/>
     <col min="13" max="13" width="22" customWidth="1"/>
-    <col min="14" max="14" width="39.33203125" customWidth="1"/>
+    <col min="14" max="14" width="32.77734375" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -704,7 +743,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -716,7 +755,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>7</v>
@@ -725,35 +764,38 @@
         <v>8</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="O1" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="12">
+      <c r="B2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="16">
         <v>0.35</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="15">
         <v>4</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="15">
         <v>8</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="15">
         <v>1</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="15" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="5">
@@ -766,120 +808,132 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+    <row r="3" spans="1:15" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="5">
         <v>2</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="16.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+    <row r="4" spans="1:15" ht="16.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="5">
         <v>1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9">
+    <row r="5" spans="1:15" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15">
         <v>2</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="11">
+        <v>23</v>
+      </c>
+      <c r="K5" s="10">
         <v>4.8899999999999997</v>
       </c>
       <c r="L5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10">
+      <c r="O5" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="9">
         <v>0.6</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K6" s="3">
         <v>19.22</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L7" s="18"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N12" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="G2:G6"/>
+    <mergeCell ref="H2:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="D2:D6"/>
     <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="F2:F6"/>
-    <mergeCell ref="G2:G6"/>
-    <mergeCell ref="H2:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -887,10 +941,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A28AAFC-1BB1-4867-BB1A-EB164CA9FEF7}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,12 +962,12 @@
     <col min="13" max="13" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -925,7 +979,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -943,35 +997,35 @@
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="141" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+    <row r="2" spans="1:14" ht="141" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="15">
         <v>400</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="17">
         <v>0.35</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="15">
         <v>16</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="15">
         <v>8</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="15">
         <v>1</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="15" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="5">
@@ -981,24 +1035,24 @@
         <v>9.34</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="3">
         <v>2</v>
       </c>
@@ -1006,37 +1060,39 @@
         <v>10.039999999999999</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:13" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+        <v>30</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:14" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
         <v>1</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="15">
         <v>400</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="17">
         <v>0.3</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="15">
         <v>16</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="15">
         <v>8</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="15">
         <v>1</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="5">
@@ -1046,24 +1102,24 @@
         <v>9.34</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="125.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+    </row>
+    <row r="6" spans="1:14" ht="125.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="3">
         <v>2</v>
       </c>
@@ -1071,23 +1127,27 @@
         <v>9.08</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K10" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>16</v>
+      </c>
+      <c r="L16">
+        <v>16</v>
+      </c>
+      <c r="M16">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1115,9 +1175,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A7818B-CA56-4EA6-9254-77ECEF653406}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1125,76 +1185,85 @@
   <cols>
     <col min="1" max="1" width="76.77734375" customWidth="1"/>
     <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="15"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>